<commit_message>
Updated with and without spare in 10th frame test cases
</commit_message>
<xml_diff>
--- a/test/BowlingGame_UnitTest.xlsx
+++ b/test/BowlingGame_UnitTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\AI\BowlingCode_IAV\BowlingGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\khay\BGUpdate\BowlingGame\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D43A0E-41BF-4BE9-A121-8DB586F57EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C3130E-7FA0-4D44-AF67-F28732FAF3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7A77D905-5FEB-4A0D-B8B3-EF42C5ED7312}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Bowling Game Unit Test Plan</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>rolls = {1,4,4,5,6,4,5,5,10,0,1,7,3,6,4,10,2,8,6}</t>
+  </si>
+  <si>
+    <t>With Spare in 10th frame</t>
+  </si>
+  <si>
+    <t>rolls = {2,4,3,6,4,5,7,2,3,5,10,0,1,7,3,4,5,9,0}</t>
+  </si>
+  <si>
+    <t>Without Spare in 10th frame</t>
   </si>
 </sst>
 </file>
@@ -140,7 +149,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -212,13 +221,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -228,13 +266,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BAAAB80-C517-420C-A4F8-01E1B9398A64}">
-  <dimension ref="C6:P19"/>
+  <dimension ref="C6:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -562,201 +600,184 @@
     <col min="5" max="5" width="39.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7265625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="C6" s="2" t="s">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="C9" s="8" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C7" s="1"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C8" s="1"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="C10" s="8" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="C11" s="8" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="C14" s="8" t="s">
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C12" s="1"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C13" s="1"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="C15" s="9" t="s">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="4">
         <v>300</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-    </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="C16" s="9" t="s">
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="4">
         <v>155</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="4">
         <v>133</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
+      <c r="E18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="4">
+        <v>85</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="D9:I9"/>
     <mergeCell ref="D10:I10"/>
     <mergeCell ref="D11:I11"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>